<commit_message>
small glitch in one user question
</commit_message>
<xml_diff>
--- a/PL 23SL01000137 Dubai AE.xlsx
+++ b/PL 23SL01000137 Dubai AE.xlsx
@@ -1251,7 +1251,7 @@
       </c>
       <c r="E20" s="32" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 ctn  120x50x30 cm </t>
+          <t xml:space="preserve">1 ctn  1x1x1 cm </t>
         </is>
       </c>
     </row>
@@ -1475,7 +1475,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.18</v>
+        <v>1e-06</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>

</xml_diff>